<commit_message>
customer maintenance page updated
</commit_message>
<xml_diff>
--- a/src/main/resources/ClientPortal_Data.xlsx
+++ b/src/main/resources/ClientPortal_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intellij Files\MAS_FloraFire\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23DF79B-FDA1-41B6-A996-4DF5CE832F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C24889-E034-4724-ACE3-684ED82BE159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2121,22 +2121,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="E48:E51"/>
     <mergeCell ref="E52:E55"/>
     <mergeCell ref="E23:E27"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E32:E35"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
message shortcut page updated
</commit_message>
<xml_diff>
--- a/src/main/resources/ClientPortal_Data.xlsx
+++ b/src/main/resources/ClientPortal_Data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS01361\My Folder\0. Test Type\4. Automation Testing\Selenium Files\MAS_FloraFire\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5E701C-0F06-4AF9-84CE-DE4FBECF5A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2578B750-71A9-4A52-890D-B3A2604FDE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
     <sheet name="ValueList" sheetId="1" r:id="rId2"/>
     <sheet name="Customer" sheetId="4" r:id="rId3"/>
+    <sheet name="ShortCuts" sheetId="6" r:id="rId4"/>
+    <sheet name="Test" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -468,6 +470,78 @@
   </si>
   <si>
     <t>william@gmail.com</t>
+  </si>
+  <si>
+    <t>Short Code</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>AML</t>
+  </si>
+  <si>
+    <t>All My Love</t>
+  </si>
+  <si>
+    <t>AOL</t>
+  </si>
+  <si>
+    <t>All Our Love</t>
+  </si>
+  <si>
+    <t>All the Best</t>
+  </si>
+  <si>
+    <t>ATB</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Best Regards</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>Best Wishes</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>Congratulations</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Deepest Sympathy</t>
+  </si>
+  <si>
+    <t>FBS</t>
+  </si>
+  <si>
+    <t>Feel Better Soon</t>
+  </si>
+  <si>
+    <t>GBY</t>
+  </si>
+  <si>
+    <t>God Bless You</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>Good Luck</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test 2</t>
   </si>
 </sst>
 </file>
@@ -2136,22 +2210,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="E48:E51"/>
     <mergeCell ref="E52:E55"/>
     <mergeCell ref="E23:E27"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E32:E35"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2162,7 +2236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75B8A7D-056B-43CF-B8CF-47A9850E51E0}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2619,4 +2693,158 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B997F-3DC4-4C7D-9993-70026FD21600}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE96B074-BAA6-41E4-A885-01589CFEB352}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gift card page added
</commit_message>
<xml_diff>
--- a/src/main/resources/ClientPortal_Data.xlsx
+++ b/src/main/resources/ClientPortal_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS01361\My Folder\0. Test Type\4. Automation Testing\Selenium Files\MAS_FloraFire\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E50F78-B047-4DAE-A632-B4D583B921D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46082E1-0BDA-4A20-BC66-873C78653560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="ShortCuts" sheetId="6" r:id="rId4"/>
     <sheet name="Vehicle" sheetId="7" r:id="rId5"/>
     <sheet name="Product" sheetId="8" r:id="rId6"/>
-    <sheet name="Test" sheetId="9" r:id="rId7"/>
+    <sheet name="GiftCard" sheetId="10" r:id="rId7"/>
+    <sheet name="Test" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="355">
   <si>
     <t>Name</t>
   </si>
@@ -1072,6 +1073,30 @@
   </si>
   <si>
     <t>03/01/2025</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Promotional</t>
+  </si>
+  <si>
+    <t>5/31/2025</t>
+  </si>
+  <si>
+    <t>6/30/2025</t>
   </si>
 </sst>
 </file>
@@ -2789,7 +2814,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5122,388 +5147,248 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4548CEF1-DD61-4E8C-BA1C-F0593B90F5FF}">
-  <dimension ref="A1:AL3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6C325F-4A76-431C-998A-38D75363C07E}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1001</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="19">
+        <v>500</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="19">
+        <v>500</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1003</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1004</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1005</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1006</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4548CEF1-DD61-4E8C-BA1C-F0593B90F5FF}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="17" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" style="17" customWidth="1"/>
     <col min="7" max="7" width="11.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.109375" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.77734375" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.77734375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="21.77734375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" style="1" customWidth="1"/>
-    <col min="35" max="35" width="12" style="1" customWidth="1"/>
-    <col min="36" max="36" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="62.21875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="12.21875" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>128</v>
+        <v>347</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>204</v>
-      </c>
       <c r="F1" s="13" t="s">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="AC1" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="AF1" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="AG1" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="AH1" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="AK1" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>58</v>
+        <v>142</v>
+      </c>
+      <c r="B2" s="19">
+        <v>2002</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" s="19">
-        <v>29.99</v>
-      </c>
-      <c r="T2" s="19">
-        <v>39.99</v>
-      </c>
-      <c r="U2" s="19">
-        <v>49.99</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="19">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="AC2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF2" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH2" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="AI2" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="AJ2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="S3" s="19">
-        <v>4.99</v>
-      </c>
-      <c r="T3" s="19">
-        <v>6.99</v>
-      </c>
-      <c r="U3" s="19">
-        <v>8.99</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="19">
-        <v>200</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="AC3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15" t="s">
-        <v>340</v>
+      <c r="F2" s="19">
+        <v>500</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
credit card settings added
</commit_message>
<xml_diff>
--- a/src/main/resources/ClientPortal_Data.xlsx
+++ b/src/main/resources/ClientPortal_Data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS01361\My Folder\0. Test Type\4. Automation Testing\Selenium Files\MAS_FloraFire\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD85706-CAAD-4198-97F3-767AE9FAFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4B57B2-323C-42A4-8C91-7EE7E320F4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" tabRatio="803" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
     <sheet name="ValueList" sheetId="1" r:id="rId2"/>
     <sheet name="Customer" sheetId="4" r:id="rId3"/>
-    <sheet name="ShortCuts" sheetId="6" r:id="rId4"/>
-    <sheet name="Vehicle" sheetId="7" r:id="rId5"/>
-    <sheet name="Product" sheetId="8" r:id="rId6"/>
+    <sheet name="Product" sheetId="8" r:id="rId4"/>
+    <sheet name="ShortCuts" sheetId="6" r:id="rId5"/>
+    <sheet name="Vehicle" sheetId="7" r:id="rId6"/>
     <sheet name="GiftCard" sheetId="10" r:id="rId7"/>
     <sheet name="Discount" sheetId="11" r:id="rId8"/>
     <sheet name="Employee" sheetId="12" r:id="rId9"/>
@@ -3779,7 +3779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -4736,6 +4736,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E56:E57"/>
     <mergeCell ref="E58:E60"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E7"/>
@@ -4752,8 +4754,6 @@
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E32:E35"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E56:E57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -5224,285 +5224,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B997F-3DC4-4C7D-9993-70026FD21600}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE96B074-BAA6-41E4-A885-01589CFEB352}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="17.88671875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="17" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C76421E-550A-4F58-ABC5-0AC68C5F2DE6}">
   <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:AA14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7097,6 +6823,280 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B997F-3DC4-4C7D-9993-70026FD21600}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE96B074-BAA6-41E4-A885-01589CFEB352}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="17.88671875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6C325F-4A76-431C-998A-38D75363C07E}">
   <dimension ref="A1:G7"/>

</xml_diff>